<commit_message>
Inversión de tiempo Gustavo De León
</commit_message>
<xml_diff>
--- a/Inversiones de Tiempo/Inversión Tiempo - Gustavo De León.xlsx
+++ b/Inversiones de Tiempo/Inversión Tiempo - Gustavo De León.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF5EF9C6-E807-4FC5-B76C-05788C07D61D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F548C83A-1A51-4F32-B35D-44D0633D4D9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1440" windowWidth="14400" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>No.</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>No ha votado nunca, cree que sería mucho mejor hablando en tiempo el voto electrónico.</t>
+  </si>
+  <si>
+    <t>Lluvia de ideas</t>
+  </si>
+  <si>
+    <t>Preguntas</t>
+  </si>
+  <si>
+    <t>Codings</t>
+  </si>
+  <si>
+    <t>Mapa de Empatía</t>
+  </si>
+  <si>
+    <t>Diagrama de caso de uso</t>
+  </si>
+  <si>
+    <t>Descripción de caso</t>
+  </si>
+  <si>
+    <t>Diagrama de actividad</t>
   </si>
 </sst>
 </file>
@@ -103,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,6 +138,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -587,6 +610,188 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>43503</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.28125</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5">
+        <v>43503</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.28125</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.28819444444444448</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43506</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F10" s="1">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1">
+        <v>90</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="5">
+        <v>43508</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>43510</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5">
+        <v>43510</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5">
+        <v>43510</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.28125</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1">
+        <v>50</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>